<commit_message>
improved geometry of domes. Their shape looks closer to half sphere
</commit_message>
<xml_diff>
--- a/vertices.xlsx
+++ b/vertices.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programy\z.studi\ROK 6\magister\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28313386-FCCB-4795-B66A-9A22C7FA1238}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97794A4-1220-4A4D-AD6B-E3B8A4755362}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,6 +40,12 @@
     <t>0.0000</t>
   </si>
   <si>
+    <t>-0.9564</t>
+  </si>
+  <si>
+    <t>0.2921</t>
+  </si>
+  <si>
     <t>-0.9511</t>
   </si>
   <si>
@@ -49,19 +55,28 @@
     <t>-0.3090</t>
   </si>
   <si>
-    <t>-0.8750</t>
-  </si>
-  <si>
-    <t>0.2920</t>
-  </si>
-  <si>
-    <t>-0.8322</t>
-  </si>
-  <si>
-    <t>0.2704</t>
-  </si>
-  <si>
-    <t>-0.2704</t>
+    <t>-0.9096</t>
+  </si>
+  <si>
+    <t>0.2955</t>
+  </si>
+  <si>
+    <t>-0.2955</t>
+  </si>
+  <si>
+    <t>-0.8586</t>
+  </si>
+  <si>
+    <t>0.5126</t>
+  </si>
+  <si>
+    <t>-0.8166</t>
+  </si>
+  <si>
+    <t>0.2653</t>
+  </si>
+  <si>
+    <t>-0.2653</t>
   </si>
   <si>
     <t>-0.8090</t>
@@ -73,229 +88,214 @@
     <t>-0.5878</t>
   </si>
   <si>
-    <t>-0.7500</t>
-  </si>
-  <si>
-    <t>0.5133</t>
-  </si>
-  <si>
-    <t>-0.7133</t>
-  </si>
-  <si>
-    <t>0.2318</t>
-  </si>
-  <si>
-    <t>-0.2318</t>
-  </si>
-  <si>
-    <t>-0.7079</t>
-  </si>
-  <si>
-    <t>0.5143</t>
-  </si>
-  <si>
-    <t>-0.5143</t>
-  </si>
-  <si>
-    <t>-0.6250</t>
-  </si>
-  <si>
-    <t>0.6447</t>
-  </si>
-  <si>
-    <t>-0.6068</t>
-  </si>
-  <si>
-    <t>0.4408</t>
-  </si>
-  <si>
-    <t>-0.4408</t>
-  </si>
-  <si>
-    <t>-0.5944</t>
-  </si>
-  <si>
-    <t>0.1931</t>
-  </si>
-  <si>
-    <t>-0.1931</t>
+    <t>-0.7737</t>
+  </si>
+  <si>
+    <t>0.5622</t>
+  </si>
+  <si>
+    <t>-0.5622</t>
+  </si>
+  <si>
+    <t>-0.7652</t>
+  </si>
+  <si>
+    <t>0.6438</t>
+  </si>
+  <si>
+    <t>-0.7277</t>
+  </si>
+  <si>
+    <t>0.2365</t>
+  </si>
+  <si>
+    <t>-0.2365</t>
+  </si>
+  <si>
+    <t>-0.6946</t>
+  </si>
+  <si>
+    <t>0.5047</t>
+  </si>
+  <si>
+    <t>-0.5047</t>
+  </si>
+  <si>
+    <t>-0.6503</t>
+  </si>
+  <si>
+    <t>0.7597</t>
+  </si>
+  <si>
+    <t>-0.6191</t>
+  </si>
+  <si>
+    <t>0.4498</t>
+  </si>
+  <si>
+    <t>-0.4498</t>
+  </si>
+  <si>
+    <t>-0.6185</t>
+  </si>
+  <si>
+    <t>0.2010</t>
+  </si>
+  <si>
+    <t>-0.2010</t>
   </si>
   <si>
     <t>0.8090</t>
   </si>
   <si>
-    <t>0.7079</t>
-  </si>
-  <si>
-    <t>-0.5056</t>
-  </si>
-  <si>
-    <t>0.3674</t>
-  </si>
-  <si>
-    <t>-0.3674</t>
-  </si>
-  <si>
-    <t>-0.5000</t>
-  </si>
-  <si>
-    <t>0.7607</t>
-  </si>
-  <si>
-    <t>-0.4755</t>
-  </si>
-  <si>
-    <t>0.1545</t>
-  </si>
-  <si>
-    <t>-0.1545</t>
-  </si>
-  <si>
-    <t>0.6068</t>
-  </si>
-  <si>
-    <t>-0.4045</t>
-  </si>
-  <si>
-    <t>0.2939</t>
-  </si>
-  <si>
-    <t>-0.2939</t>
-  </si>
-  <si>
-    <t>-0.3750</t>
-  </si>
-  <si>
-    <t>0.8653</t>
-  </si>
-  <si>
-    <t>0.5056</t>
-  </si>
-  <si>
-    <t>-0.3566</t>
-  </si>
-  <si>
-    <t>0.1159</t>
-  </si>
-  <si>
-    <t>-0.1159</t>
+    <t>0.7737</t>
+  </si>
+  <si>
+    <t>-0.5261</t>
+  </si>
+  <si>
+    <t>0.3822</t>
+  </si>
+  <si>
+    <t>-0.3822</t>
+  </si>
+  <si>
+    <t>0.6946</t>
+  </si>
+  <si>
+    <t>-0.5031</t>
+  </si>
+  <si>
+    <t>0.8642</t>
+  </si>
+  <si>
+    <t>-0.4785</t>
+  </si>
+  <si>
+    <t>0.1555</t>
+  </si>
+  <si>
+    <t>-0.1555</t>
+  </si>
+  <si>
+    <t>0.6191</t>
+  </si>
+  <si>
+    <t>-0.4070</t>
+  </si>
+  <si>
+    <t>0.2957</t>
+  </si>
+  <si>
+    <t>-0.2957</t>
+  </si>
+  <si>
+    <t>-0.4000</t>
+  </si>
+  <si>
+    <t>0.9165</t>
+  </si>
+  <si>
+    <t>0.5261</t>
+  </si>
+  <si>
+    <t>-0.3804</t>
+  </si>
+  <si>
+    <t>0.1236</t>
+  </si>
+  <si>
+    <t>-0.1236</t>
+  </si>
+  <si>
+    <t>-0.3236</t>
+  </si>
+  <si>
+    <t>0.2351</t>
+  </si>
+  <si>
+    <t>-0.2351</t>
   </si>
   <si>
     <t>0.9511</t>
   </si>
   <si>
-    <t>-0.3034</t>
-  </si>
-  <si>
-    <t>0.2204</t>
-  </si>
-  <si>
-    <t>-0.2204</t>
-  </si>
-  <si>
-    <t>0.4045</t>
-  </si>
-  <si>
-    <t>-0.2750</t>
-  </si>
-  <si>
-    <t>0.9249</t>
-  </si>
-  <si>
-    <t>0.8322</t>
-  </si>
-  <si>
-    <t>-0.2615</t>
-  </si>
-  <si>
-    <t>0.0850</t>
-  </si>
-  <si>
-    <t>-0.0850</t>
-  </si>
-  <si>
-    <t>0.7133</t>
-  </si>
-  <si>
-    <t>-0.2225</t>
-  </si>
-  <si>
-    <t>0.1616</t>
-  </si>
-  <si>
-    <t>-0.1616</t>
-  </si>
-  <si>
-    <t>0.3034</t>
-  </si>
-  <si>
-    <t>0.5944</t>
-  </si>
-  <si>
-    <t>0.2225</t>
-  </si>
-  <si>
-    <t>0.4755</t>
-  </si>
-  <si>
-    <t>-0.1250</t>
-  </si>
-  <si>
-    <t>0.9787</t>
-  </si>
-  <si>
-    <t>-0.1189</t>
-  </si>
-  <si>
-    <t>0.0386</t>
-  </si>
-  <si>
-    <t>-0.0386</t>
-  </si>
-  <si>
-    <t>0.3566</t>
-  </si>
-  <si>
-    <t>-0.1011</t>
-  </si>
-  <si>
-    <t>0.0735</t>
-  </si>
-  <si>
-    <t>-0.0735</t>
-  </si>
-  <si>
-    <t>0.2615</t>
-  </si>
-  <si>
-    <t>0.1011</t>
-  </si>
-  <si>
-    <t>0.1189</t>
-  </si>
-  <si>
-    <t>0.5000</t>
-  </si>
-  <si>
-    <t>0.3750</t>
-  </si>
-  <si>
-    <t>0.1250</t>
-  </si>
-  <si>
-    <t>0.6250</t>
+    <t>0.4070</t>
+  </si>
+  <si>
+    <t>0.9096</t>
+  </si>
+  <si>
+    <t>0.8166</t>
+  </si>
+  <si>
+    <t>0.7277</t>
+  </si>
+  <si>
+    <t>0.3236</t>
+  </si>
+  <si>
+    <t>-0.2097</t>
+  </si>
+  <si>
+    <t>0.9778</t>
+  </si>
+  <si>
+    <t>0.6185</t>
+  </si>
+  <si>
+    <t>-0.1994</t>
+  </si>
+  <si>
+    <t>0.0648</t>
+  </si>
+  <si>
+    <t>-0.0648</t>
+  </si>
+  <si>
+    <t>-0.1697</t>
+  </si>
+  <si>
+    <t>0.1233</t>
+  </si>
+  <si>
+    <t>-0.1233</t>
+  </si>
+  <si>
+    <t>0.4785</t>
+  </si>
+  <si>
+    <t>0.3804</t>
+  </si>
+  <si>
+    <t>0.1697</t>
+  </si>
+  <si>
+    <t>0.1994</t>
+  </si>
+  <si>
+    <t>0.5031</t>
+  </si>
+  <si>
+    <t>0.6503</t>
+  </si>
+  <si>
+    <t>0.2097</t>
+  </si>
+  <si>
+    <t>0.4000</t>
+  </si>
+  <si>
+    <t>0.9564</t>
   </si>
   <si>
     <t>1.0000</t>
   </si>
   <si>
-    <t>0.8750</t>
-  </si>
-  <si>
-    <t>0.7500</t>
-  </si>
-  <si>
-    <t>0.2750</t>
+    <t>0.7652</t>
+  </si>
+  <si>
+    <t>0.8586</t>
   </si>
 </sst>
 </file>
@@ -365,7 +365,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -377,7 +377,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -424,6 +424,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -459,6 +476,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -644,18 +678,18 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -663,13 +697,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -680,7 +714,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -691,7 +725,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -699,32 +733,32 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -735,7 +769,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -746,7 +780,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -757,7 +791,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -768,7 +802,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -790,7 +824,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -801,7 +835,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -812,7 +846,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -823,150 +857,150 @@
         <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -982,238 +1016,238 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>68</v>
@@ -1224,10 +1258,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>25</v>
@@ -1235,57 +1269,57 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1296,7 +1330,7 @@
         <v>74</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -1307,95 +1341,95 @@
         <v>75</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1406,7 +1440,7 @@
         <v>82</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1417,7 +1451,7 @@
         <v>73</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1428,7 +1462,7 @@
         <v>83</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -1439,7 +1473,7 @@
         <v>84</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -1450,7 +1484,7 @@
         <v>85</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -1461,7 +1495,7 @@
         <v>86</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -1472,7 +1506,7 @@
         <v>87</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -1483,7 +1517,7 @@
         <v>88</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1494,7 +1528,7 @@
         <v>89</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -1502,10 +1536,10 @@
         <v>4</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -1513,10 +1547,10 @@
         <v>4</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -1535,10 +1569,10 @@
         <v>4</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -1546,10 +1580,10 @@
         <v>4</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -1557,10 +1591,10 @@
         <v>4</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -1568,10 +1602,10 @@
         <v>4</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -1579,10 +1613,10 @@
         <v>4</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -1590,10 +1624,10 @@
         <v>4</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -1601,10 +1635,10 @@
         <v>4</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -1615,7 +1649,7 @@
         <v>82</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -1626,95 +1660,95 @@
         <v>73</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -1725,7 +1759,7 @@
         <v>74</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -1736,67 +1770,67 @@
         <v>75</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>68</v>
@@ -1807,10 +1841,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>25</v>
@@ -1818,238 +1852,238 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>4</v>
@@ -2060,194 +2094,194 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="B141" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>4</v>
@@ -2258,120 +2292,120 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="B155" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C155" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>4</v>
@@ -2379,18 +2413,18 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>4</v>

</xml_diff>